<commit_message>
acompanhar receite use case
</commit_message>
<xml_diff>
--- a/UseCaseDescription.xlsx
+++ b/UseCaseDescription.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barbosa\Desktop\LI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1571097-1344-40C7-91AA-1B8B38E93A70}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D788134E-2026-4530-ABDE-0563CAEDE975}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
   <si>
     <t>Use Case:</t>
   </si>
@@ -117,13 +117,61 @@
   </si>
   <si>
     <t>3. Seleciona receitas que não estão no histórico do utilizador</t>
+  </si>
+  <si>
+    <t>Acompanhamento da receita</t>
+  </si>
+  <si>
+    <t>1. Indica que pretende confecionar a receita</t>
+  </si>
+  <si>
+    <t>2. Exibe próxima etapa da receita</t>
+  </si>
+  <si>
+    <t>3. Utilizador indica que completou passo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Regista estatisticas </t>
+  </si>
+  <si>
+    <t>Alternativa 1 [etapa tem limite de tempo] (passo 2)</t>
+  </si>
+  <si>
+    <t>2.1a Exibe a opção de começar um temporizador (?)</t>
+  </si>
+  <si>
+    <t>2.2a Utilizador começa temporizador</t>
+  </si>
+  <si>
+    <t>Volta a 2</t>
+  </si>
+  <si>
+    <t>Alternativa 2 [utilizador seleciona termo] (passo 2)</t>
+  </si>
+  <si>
+    <t>2.1b Exibe definição do termo selecionado</t>
+  </si>
+  <si>
+    <t>Alternativa 3 [utilizar seleciona ajuda] (passo 2)</t>
+  </si>
+  <si>
+    <t>2.1c Encaminha o utilizador para o recurso de ajuda</t>
+  </si>
+  <si>
+    <t>Alternativa 4 [ainda existem mais etapas] (passo 4)</t>
+  </si>
+  <si>
+    <t>Alternativa 5 [temporizador termina] (passo )</t>
+  </si>
+  <si>
+    <t>.1 Avisa utilizador que o tempo terminou</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -147,6 +195,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -168,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -501,11 +560,105 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -529,56 +682,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
@@ -587,9 +696,88 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -906,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D909"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -925,38 +1113,38 @@
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="18"/>
+      <c r="D4" s="35"/>
     </row>
     <row r="5" spans="2:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="18"/>
+      <c r="D5" s="35"/>
     </row>
     <row r="6" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
     </row>
     <row r="7" spans="2:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="25"/>
+      <c r="D7" s="37"/>
     </row>
     <row r="8" spans="2:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -967,21 +1155,21 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="23"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="14"/>
     </row>
     <row r="10" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="4"/>
       <c r="D10" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="23"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
@@ -999,7 +1187,7 @@
       <c r="D13" s="16"/>
     </row>
     <row r="14" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="27" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="12" t="s">
@@ -1008,12 +1196,12 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="21"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="13"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="27" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="12"/>
@@ -1022,7 +1210,7 @@
       </c>
     </row>
     <row r="17" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="21"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="13"/>
       <c r="D17" s="3"/>
     </row>
@@ -1033,38 +1221,38 @@
       <c r="B21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="18"/>
+      <c r="D21" s="35"/>
     </row>
     <row r="22" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="18"/>
+      <c r="D22" s="35"/>
     </row>
     <row r="23" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="35"/>
     </row>
     <row r="24" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="25"/>
+      <c r="D24" s="37"/>
     </row>
     <row r="25" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -1075,21 +1263,21 @@
       </c>
     </row>
     <row r="26" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="27"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="14"/>
     </row>
     <row r="27" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="27"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="4"/>
       <c r="D27" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="27"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="4" t="s">
         <v>11</v>
       </c>
@@ -1109,7 +1297,7 @@
       </c>
     </row>
     <row r="31" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="27" t="s">
         <v>20</v>
       </c>
       <c r="C31" s="12"/>
@@ -1118,7 +1306,7 @@
       </c>
     </row>
     <row r="32" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="26"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="13"/>
       <c r="D32" s="3"/>
     </row>
@@ -1126,110 +1314,248 @@
     <row r="34" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="30"/>
+      <c r="D36" s="32"/>
     </row>
     <row r="37" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D37" s="30"/>
+      <c r="D37" s="32"/>
     </row>
     <row r="38" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="29" t="s">
+      <c r="C38" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="D38" s="30"/>
+      <c r="D38" s="32"/>
     </row>
     <row r="39" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="31" t="s">
+      <c r="C39" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="32"/>
+      <c r="D39" s="39"/>
     </row>
     <row r="40" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="40" t="s">
+      <c r="B40" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="33" t="s">
+      <c r="C40" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="34" t="s">
+      <c r="D40" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="35"/>
-      <c r="C41" s="36" t="s">
+      <c r="B41" s="25"/>
+      <c r="C41" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="37"/>
+      <c r="D41" s="21"/>
     </row>
     <row r="42" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="35"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="37" t="s">
+      <c r="B42" s="25"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="21" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="41"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="38" t="s">
+      <c r="B43" s="26"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="22" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" s="35"/>
+    </row>
+    <row r="48" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="35"/>
+    </row>
+    <row r="49" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="42"/>
+      <c r="D49" s="43"/>
+    </row>
+    <row r="50" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="44"/>
+      <c r="D50" s="45"/>
+    </row>
+    <row r="51" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="30"/>
+      <c r="C52" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" s="49"/>
+    </row>
+    <row r="53" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="30"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="51" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="30"/>
+      <c r="C54" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="D54" s="51"/>
+    </row>
+    <row r="55" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="7"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="51" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="53"/>
+      <c r="C56" s="54"/>
+      <c r="D56" s="55"/>
+    </row>
+    <row r="57" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C57" s="56"/>
+      <c r="D57" s="57" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="58"/>
+      <c r="C58" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="D58" s="51"/>
+    </row>
+    <row r="59" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="40"/>
+      <c r="C59" s="54"/>
+      <c r="D59" s="55" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="56"/>
+      <c r="D60" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="28"/>
+      <c r="C61" s="59"/>
+      <c r="D61" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" s="60"/>
+      <c r="D62" s="61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="28"/>
+      <c r="C63" s="59"/>
+      <c r="D63" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C64" s="60"/>
+      <c r="D64" s="62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="28"/>
+      <c r="C65" s="59"/>
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C66" s="60"/>
+      <c r="D66" s="62" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="28"/>
+      <c r="C67" s="59"/>
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1253,20 +1579,20 @@
     <row r="101" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="102" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="103" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C103" s="19"/>
-      <c r="D103" s="19"/>
+      <c r="C103" s="33"/>
+      <c r="D103" s="33"/>
     </row>
     <row r="104" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C104" s="19"/>
-      <c r="D104" s="19"/>
+      <c r="C104" s="33"/>
+      <c r="D104" s="33"/>
     </row>
     <row r="105" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C105" s="19"/>
-      <c r="D105" s="19"/>
+      <c r="C105" s="33"/>
+      <c r="D105" s="33"/>
     </row>
     <row r="106" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C106" s="19"/>
-      <c r="D106" s="19"/>
+      <c r="C106" s="33"/>
+      <c r="D106" s="33"/>
     </row>
     <row r="107" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C107" s="5"/>
@@ -1319,20 +1645,20 @@
     <row r="119" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="120" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="121" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C121" s="19"/>
-      <c r="D121" s="19"/>
+      <c r="C121" s="33"/>
+      <c r="D121" s="33"/>
     </row>
     <row r="122" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C122" s="19"/>
-      <c r="D122" s="19"/>
+      <c r="C122" s="33"/>
+      <c r="D122" s="33"/>
     </row>
     <row r="123" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C123" s="19"/>
-      <c r="D123" s="19"/>
+      <c r="C123" s="33"/>
+      <c r="D123" s="33"/>
     </row>
     <row r="124" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C124" s="19"/>
-      <c r="D124" s="19"/>
+      <c r="C124" s="33"/>
+      <c r="D124" s="33"/>
     </row>
     <row r="125" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C125" s="5"/>
@@ -2136,13 +2462,29 @@
     <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="26">
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
+  <mergeCells count="36">
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="C121:D121"/>
     <mergeCell ref="C123:D123"/>
     <mergeCell ref="C124:D124"/>
@@ -2151,18 +2493,12 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C39:D39"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>